<commit_message>
Added series of images calculatation
wavelength_calculation_series.py - modifed wavelength_calculation.py to calculate the wavelengths for a a series of images. Saving the wavelengths and intensities for all detected particles at the first frame of the series.
</commit_message>
<xml_diff>
--- a/X2110-Camera/100x/beads-6/center-sigma-green-3.xlsx
+++ b/X2110-Camera/100x/beads-6/center-sigma-green-3.xlsx
@@ -15,12 +15,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>centers</t>
   </si>
   <si>
     <t>sigmas</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>588.2324014377622</t>
+  </si>
+  <si>
+    <t>20.483870684032574</t>
+  </si>
+  <si>
+    <t>lorentzian</t>
+  </si>
+  <si>
+    <t>590.579897700339</t>
+  </si>
+  <si>
+    <t>23.020675159970697</t>
+  </si>
+  <si>
+    <t>588.4651556167944</t>
+  </si>
+  <si>
+    <t>29.011885913097565</t>
+  </si>
+  <si>
+    <t>587.410328949432</t>
+  </si>
+  <si>
+    <t>30.051801152240728</t>
+  </si>
+  <si>
+    <t>586.9501731057403</t>
+  </si>
+  <si>
+    <t>26.405473968522095</t>
+  </si>
+  <si>
+    <t>585.8396267334707</t>
+  </si>
+  <si>
+    <t>22.8898502379652</t>
+  </si>
+  <si>
+    <t>583.2124706812614</t>
+  </si>
+  <si>
+    <t>31.521944504049202</t>
+  </si>
+  <si>
+    <t>584.5742851192283</t>
+  </si>
+  <si>
+    <t>38.983418655530954</t>
+  </si>
+  <si>
+    <t>581.4196673282353</t>
+  </si>
+  <si>
+    <t>30.502261739669603</t>
   </si>
 </sst>
 </file>
@@ -369,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -377,111 +437,141 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>588.2324014377622</v>
-      </c>
-      <c r="C2" t="n">
-        <v>20.48387068403257</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>590.579897700339</v>
-      </c>
-      <c r="C3" t="n">
-        <v>23.0206751599707</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>588.4651556167944</v>
-      </c>
-      <c r="C4" t="n">
-        <v>29.01188591309757</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
-        <v>587.410328949432</v>
-      </c>
-      <c r="C5" t="n">
-        <v>30.05180115224073</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
-        <v>586.9501731057403</v>
-      </c>
-      <c r="C6" t="n">
-        <v>26.4054739685221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
-        <v>585.8396267334707</v>
-      </c>
-      <c r="C7" t="n">
-        <v>22.8898502379652</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
-        <v>583.2124706812614</v>
-      </c>
-      <c r="C8" t="n">
-        <v>31.5219445040492</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
-        <v>584.5742851192283</v>
-      </c>
-      <c r="C9" t="n">
-        <v>38.98341865553095</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
-        <v>581.4196673282353</v>
-      </c>
-      <c r="C10" t="n">
-        <v>30.5022617396696</v>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>